<commit_message>
Changed target generation to include p.populatin and star catalog separately
</commit_message>
<xml_diff>
--- a/GUI_Backend/gui_input.xlsx
+++ b/GUI_Backend/gui_input.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rpatel/Dropbox (Personal)/Research/WFIRST/EXOSIMSTesting/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anakha272\Dropbox (Personal)\Research\WFIRST\EXOSIMSTesting\GUI_Backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11640" yWindow="1260" windowWidth="26760" windowHeight="22660" tabRatio="500"/>
+    <workbookView xWindow="11640" yWindow="1260" windowWidth="26760" windowHeight="22665" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="105">
   <si>
     <t>Input Variable</t>
   </si>
@@ -53,9 +53,6 @@
     <t>magnitudes</t>
   </si>
   <si>
-    <t>Target List</t>
-  </si>
-  <si>
     <t>Variable Name</t>
   </si>
   <si>
@@ -101,9 +98,6 @@
     <t>Mission Parameters</t>
   </si>
   <si>
-    <t>Built in Targets</t>
-  </si>
-  <si>
     <t>Central Wavelength</t>
   </si>
   <si>
@@ -318,13 +312,43 @@
   </si>
   <si>
     <t>Optical system overhead time in units of days.</t>
+  </si>
+  <si>
+    <t>Target Generation</t>
+  </si>
+  <si>
+    <t>Planet Population</t>
+  </si>
+  <si>
+    <t>Earth Twin Hab Planets</t>
+  </si>
+  <si>
+    <t>EarthTwin</t>
+  </si>
+  <si>
+    <t>Star Catalog</t>
+  </si>
+  <si>
+    <t>EXOCAT</t>
+  </si>
+  <si>
+    <t>SIMBAD Catalog</t>
+  </si>
+  <si>
+    <t>-CatType</t>
+  </si>
+  <si>
+    <t>EXOCAT1</t>
+  </si>
+  <si>
+    <t>SIMBADCatalog</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -592,7 +616,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -689,9 +713,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -701,28 +749,19 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1098,52 +1137,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R60"/>
+  <dimension ref="A1:R63"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="113" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" customWidth="1"/>
-    <col min="5" max="5" width="0.6640625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="0.6640625" style="7" customWidth="1"/>
-    <col min="7" max="7" width="47.6640625" style="27" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.5" customWidth="1"/>
-    <col min="9" max="9" width="1.1640625" customWidth="1"/>
+    <col min="2" max="2" width="20.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="0.625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="0.625" style="7" customWidth="1"/>
+    <col min="7" max="7" width="17.5" style="27" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.375" customWidth="1"/>
+    <col min="9" max="9" width="1.125" customWidth="1"/>
     <col min="10" max="17" width="11" style="55"/>
-    <col min="18" max="18" width="55.1640625" style="55" customWidth="1"/>
+    <col min="18" max="18" width="69" style="55" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="56" t="s">
-        <v>39</v>
-      </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
+    <row r="1" spans="1:18" ht="23.25">
+      <c r="A1" s="58" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
       <c r="E1" s="5"/>
-      <c r="G1" s="57" t="s">
+      <c r="G1" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="58"/>
+      <c r="H1" s="66"/>
       <c r="I1" s="49"/>
-      <c r="J1" s="65" t="s">
-        <v>76</v>
-      </c>
-      <c r="K1" s="56"/>
-      <c r="L1" s="56"/>
-      <c r="M1" s="56"/>
-      <c r="N1" s="56"/>
-      <c r="O1" s="56"/>
-      <c r="P1" s="56"/>
-      <c r="Q1" s="56"/>
-      <c r="R1" s="66"/>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="J1" s="57" t="s">
+        <v>74</v>
+      </c>
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="58"/>
+      <c r="O1" s="58"/>
+      <c r="P1" s="58"/>
+      <c r="Q1" s="58"/>
+      <c r="R1" s="59"/>
+    </row>
+    <row r="2" spans="1:18">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1154,26 +1194,26 @@
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G2" s="23" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I2" s="50"/>
-      <c r="J2" s="67"/>
-      <c r="K2" s="67"/>
-      <c r="L2" s="67"/>
-      <c r="M2" s="67"/>
-      <c r="N2" s="67"/>
-      <c r="O2" s="67"/>
-      <c r="P2" s="67"/>
-      <c r="Q2" s="67"/>
-      <c r="R2" s="67"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="J2" s="60"/>
+      <c r="K2" s="60"/>
+      <c r="L2" s="60"/>
+      <c r="M2" s="60"/>
+      <c r="N2" s="60"/>
+      <c r="O2" s="60"/>
+      <c r="P2" s="60"/>
+      <c r="Q2" s="60"/>
+      <c r="R2" s="60"/>
+    </row>
+    <row r="3" spans="1:18">
       <c r="G3" s="46"/>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
@@ -1187,19 +1227,19 @@
       <c r="Q3" s="1"/>
       <c r="R3" s="7"/>
     </row>
-    <row r="4" spans="1:18" ht="19" x14ac:dyDescent="0.2">
-      <c r="A4" s="59" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="59"/>
-      <c r="C4" s="59"/>
-      <c r="D4" s="60"/>
+    <row r="4" spans="1:18" ht="18.75">
+      <c r="A4" s="67" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="67"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="63"/>
       <c r="E4" s="8"/>
       <c r="F4" s="9"/>
-      <c r="G4" s="61" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="60"/>
+      <c r="G4" s="62" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="63"/>
       <c r="I4" s="51"/>
       <c r="J4" s="6"/>
       <c r="K4" s="1"/>
@@ -1211,7 +1251,7 @@
       <c r="Q4" s="1"/>
       <c r="R4" s="7"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18">
       <c r="G5" s="46"/>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
@@ -1225,7 +1265,7 @@
       <c r="Q5" s="1"/>
       <c r="R5" s="7"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18">
       <c r="A6" s="10" t="s">
         <v>2</v>
       </c>
@@ -1236,62 +1276,62 @@
         <v>6</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G6" s="24" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H6" s="36" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I6" s="7"/>
-      <c r="J6" s="62" t="s">
-        <v>77</v>
-      </c>
-      <c r="K6" s="62"/>
-      <c r="L6" s="62"/>
-      <c r="M6" s="62"/>
-      <c r="N6" s="62"/>
-      <c r="O6" s="62"/>
-      <c r="P6" s="62"/>
-      <c r="Q6" s="62"/>
-      <c r="R6" s="62"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="J6" s="61" t="s">
+        <v>75</v>
+      </c>
+      <c r="K6" s="61"/>
+      <c r="L6" s="61"/>
+      <c r="M6" s="61"/>
+      <c r="N6" s="61"/>
+      <c r="O6" s="61"/>
+      <c r="P6" s="61"/>
+      <c r="Q6" s="61"/>
+      <c r="R6" s="61"/>
+    </row>
+    <row r="7" spans="1:18">
       <c r="A7" s="14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="15">
         <v>0.16669999999999999</v>
       </c>
       <c r="C7" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="7"/>
+      <c r="J7" s="56" t="s">
+        <v>76</v>
+      </c>
+      <c r="K7" s="56"/>
+      <c r="L7" s="56"/>
+      <c r="M7" s="56"/>
+      <c r="N7" s="56"/>
+      <c r="O7" s="56"/>
+      <c r="P7" s="56"/>
+      <c r="Q7" s="56"/>
+      <c r="R7" s="56"/>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="A8" s="14" t="s">
         <v>11</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="G7" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="H7" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="I7" s="7"/>
-      <c r="J7" s="64" t="s">
-        <v>78</v>
-      </c>
-      <c r="K7" s="64"/>
-      <c r="L7" s="64"/>
-      <c r="M7" s="64"/>
-      <c r="N7" s="64"/>
-      <c r="O7" s="64"/>
-      <c r="P7" s="64"/>
-      <c r="Q7" s="64"/>
-      <c r="R7" s="64"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A8" s="14" t="s">
-        <v>12</v>
       </c>
       <c r="B8" s="15">
         <v>0</v>
@@ -1300,60 +1340,60 @@
         <v>6</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G8" s="25" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H8" s="43" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I8" s="7"/>
-      <c r="J8" s="64" t="s">
-        <v>79</v>
-      </c>
-      <c r="K8" s="64"/>
-      <c r="L8" s="64"/>
-      <c r="M8" s="64"/>
-      <c r="N8" s="64"/>
-      <c r="O8" s="64"/>
-      <c r="P8" s="64"/>
-      <c r="Q8" s="64"/>
-      <c r="R8" s="64"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="J8" s="56" t="s">
+        <v>77</v>
+      </c>
+      <c r="K8" s="56"/>
+      <c r="L8" s="56"/>
+      <c r="M8" s="56"/>
+      <c r="N8" s="56"/>
+      <c r="O8" s="56"/>
+      <c r="P8" s="56"/>
+      <c r="Q8" s="56"/>
+      <c r="R8" s="56"/>
+    </row>
+    <row r="9" spans="1:18">
       <c r="A9" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" s="15">
         <v>60676</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G9" s="25" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H9" s="43" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I9" s="7"/>
-      <c r="J9" s="64" t="s">
-        <v>80</v>
-      </c>
-      <c r="K9" s="64"/>
-      <c r="L9" s="64"/>
-      <c r="M9" s="64"/>
-      <c r="N9" s="64"/>
-      <c r="O9" s="64"/>
-      <c r="P9" s="64"/>
-      <c r="Q9" s="64"/>
-      <c r="R9" s="64"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="J9" s="56" t="s">
+        <v>78</v>
+      </c>
+      <c r="K9" s="56"/>
+      <c r="L9" s="56"/>
+      <c r="M9" s="56"/>
+      <c r="N9" s="56"/>
+      <c r="O9" s="56"/>
+      <c r="P9" s="56"/>
+      <c r="Q9" s="56"/>
+      <c r="R9" s="56"/>
+    </row>
+    <row r="10" spans="1:18">
       <c r="A10" s="14" t="s">
         <v>4</v>
       </c>
@@ -1364,296 +1404,296 @@
         <v>7</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G10" s="25" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H10" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="7"/>
+      <c r="J10" s="56" t="s">
+        <v>79</v>
+      </c>
+      <c r="K10" s="56"/>
+      <c r="L10" s="56"/>
+      <c r="M10" s="56"/>
+      <c r="N10" s="56"/>
+      <c r="O10" s="56"/>
+      <c r="P10" s="56"/>
+      <c r="Q10" s="56"/>
+      <c r="R10" s="56"/>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="A11" s="18" t="s">
         <v>16</v>
-      </c>
-      <c r="I10" s="7"/>
-      <c r="J10" s="64" t="s">
-        <v>81</v>
-      </c>
-      <c r="K10" s="64"/>
-      <c r="L10" s="64"/>
-      <c r="M10" s="64"/>
-      <c r="N10" s="64"/>
-      <c r="O10" s="64"/>
-      <c r="P10" s="64"/>
-      <c r="Q10" s="64"/>
-      <c r="R10" s="64"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A11" s="18" t="s">
-        <v>17</v>
       </c>
       <c r="B11" s="19">
         <v>0.02</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G11" s="26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H11" s="22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I11" s="7"/>
-      <c r="J11" s="64" t="s">
-        <v>82</v>
-      </c>
-      <c r="K11" s="64"/>
-      <c r="L11" s="64"/>
-      <c r="M11" s="64"/>
-      <c r="N11" s="64"/>
-      <c r="O11" s="64"/>
-      <c r="P11" s="64"/>
-      <c r="Q11" s="64"/>
-      <c r="R11" s="64"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="J11" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="K11" s="56"/>
+      <c r="L11" s="56"/>
+      <c r="M11" s="56"/>
+      <c r="N11" s="56"/>
+      <c r="O11" s="56"/>
+      <c r="P11" s="56"/>
+      <c r="Q11" s="56"/>
+      <c r="R11" s="56"/>
+    </row>
+    <row r="12" spans="1:18">
       <c r="A12" s="14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B12" s="15">
         <v>0.02</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G12" s="25" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H12" s="43" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I12" s="7"/>
-      <c r="J12" s="64" t="s">
-        <v>83</v>
-      </c>
-      <c r="K12" s="64"/>
-      <c r="L12" s="64"/>
-      <c r="M12" s="64"/>
-      <c r="N12" s="64"/>
-      <c r="O12" s="64"/>
-      <c r="P12" s="64"/>
-      <c r="Q12" s="64"/>
-      <c r="R12" s="64"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="J12" s="56" t="s">
+        <v>81</v>
+      </c>
+      <c r="K12" s="56"/>
+      <c r="L12" s="56"/>
+      <c r="M12" s="56"/>
+      <c r="N12" s="56"/>
+      <c r="O12" s="56"/>
+      <c r="P12" s="56"/>
+      <c r="Q12" s="56"/>
+      <c r="R12" s="56"/>
+    </row>
+    <row r="13" spans="1:18">
       <c r="A13" s="32" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B13" s="37">
         <v>10</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D13" s="34" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E13" s="35"/>
       <c r="F13" s="36"/>
       <c r="G13" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="H13" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" s="7"/>
+      <c r="J13" s="56" t="s">
+        <v>82</v>
+      </c>
+      <c r="K13" s="56"/>
+      <c r="L13" s="56"/>
+      <c r="M13" s="56"/>
+      <c r="N13" s="56"/>
+      <c r="O13" s="56"/>
+      <c r="P13" s="56"/>
+      <c r="Q13" s="56"/>
+      <c r="R13" s="56"/>
+    </row>
+    <row r="14" spans="1:18">
+      <c r="A14" s="38" t="s">
         <v>61</v>
-      </c>
-      <c r="H13" s="47" t="s">
-        <v>16</v>
-      </c>
-      <c r="I13" s="7"/>
-      <c r="J13" s="64" t="s">
-        <v>84</v>
-      </c>
-      <c r="K13" s="64"/>
-      <c r="L13" s="64"/>
-      <c r="M13" s="64"/>
-      <c r="N13" s="64"/>
-      <c r="O13" s="64"/>
-      <c r="P13" s="64"/>
-      <c r="Q13" s="64"/>
-      <c r="R13" s="64"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A14" s="38" t="s">
-        <v>63</v>
       </c>
       <c r="B14" s="39">
         <v>30</v>
       </c>
       <c r="C14" s="40" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D14" s="41" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E14" s="42"/>
       <c r="F14" s="43"/>
       <c r="G14" s="25" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H14" s="48" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I14" s="7"/>
-      <c r="J14" s="64" t="s">
-        <v>85</v>
-      </c>
-      <c r="K14" s="64"/>
-      <c r="L14" s="64"/>
-      <c r="M14" s="64"/>
-      <c r="N14" s="64"/>
-      <c r="O14" s="64"/>
-      <c r="P14" s="64"/>
-      <c r="Q14" s="64"/>
-      <c r="R14" s="64"/>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="J14" s="56" t="s">
+        <v>83</v>
+      </c>
+      <c r="K14" s="56"/>
+      <c r="L14" s="56"/>
+      <c r="M14" s="56"/>
+      <c r="N14" s="56"/>
+      <c r="O14" s="56"/>
+      <c r="P14" s="56"/>
+      <c r="Q14" s="56"/>
+      <c r="R14" s="56"/>
+    </row>
+    <row r="15" spans="1:18">
       <c r="A15" s="38" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B15" s="39">
         <v>0.1</v>
       </c>
       <c r="C15" s="40" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D15" s="41" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E15" s="42"/>
       <c r="F15" s="43"/>
       <c r="G15" s="25" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H15" s="48" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I15" s="7"/>
-      <c r="J15" s="64" t="s">
-        <v>86</v>
-      </c>
-      <c r="K15" s="64"/>
-      <c r="L15" s="64"/>
-      <c r="M15" s="64"/>
-      <c r="N15" s="64"/>
-      <c r="O15" s="64"/>
-      <c r="P15" s="64"/>
-      <c r="Q15" s="64"/>
-      <c r="R15" s="64"/>
-    </row>
-    <row r="16" spans="1:18" ht="19" x14ac:dyDescent="0.2">
+      <c r="J15" s="56" t="s">
+        <v>84</v>
+      </c>
+      <c r="K15" s="56"/>
+      <c r="L15" s="56"/>
+      <c r="M15" s="56"/>
+      <c r="N15" s="56"/>
+      <c r="O15" s="56"/>
+      <c r="P15" s="56"/>
+      <c r="Q15" s="56"/>
+      <c r="R15" s="56"/>
+    </row>
+    <row r="16" spans="1:18" ht="18.75">
       <c r="A16" s="38" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B16" s="39">
         <v>0.3</v>
       </c>
       <c r="C16" s="40" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D16" s="41" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E16" s="42"/>
       <c r="F16" s="43"/>
       <c r="G16" s="25" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H16" s="48" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I16" s="51"/>
-      <c r="J16" s="64" t="s">
-        <v>87</v>
-      </c>
-      <c r="K16" s="64"/>
-      <c r="L16" s="64"/>
-      <c r="M16" s="64"/>
-      <c r="N16" s="64"/>
-      <c r="O16" s="64"/>
-      <c r="P16" s="64"/>
-      <c r="Q16" s="64"/>
-      <c r="R16" s="64"/>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="J16" s="56" t="s">
+        <v>85</v>
+      </c>
+      <c r="K16" s="56"/>
+      <c r="L16" s="56"/>
+      <c r="M16" s="56"/>
+      <c r="N16" s="56"/>
+      <c r="O16" s="56"/>
+      <c r="P16" s="56"/>
+      <c r="Q16" s="56"/>
+      <c r="R16" s="56"/>
+    </row>
+    <row r="17" spans="1:18">
       <c r="A17" s="38" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B17" s="44">
         <v>2.9999999999999999E-7</v>
       </c>
       <c r="C17" s="40" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D17" s="41" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E17" s="42"/>
       <c r="F17" s="43"/>
       <c r="G17" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="H17" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="I17" s="7"/>
+      <c r="J17" s="56" t="s">
+        <v>86</v>
+      </c>
+      <c r="K17" s="56"/>
+      <c r="L17" s="56"/>
+      <c r="M17" s="56"/>
+      <c r="N17" s="56"/>
+      <c r="O17" s="56"/>
+      <c r="P17" s="56"/>
+      <c r="Q17" s="56"/>
+      <c r="R17" s="56"/>
+    </row>
+    <row r="18" spans="1:18">
+      <c r="A18" s="38" t="s">
         <v>69</v>
-      </c>
-      <c r="H17" s="48" t="s">
-        <v>16</v>
-      </c>
-      <c r="I17" s="7"/>
-      <c r="J17" s="64" t="s">
-        <v>88</v>
-      </c>
-      <c r="K17" s="64"/>
-      <c r="L17" s="64"/>
-      <c r="M17" s="64"/>
-      <c r="N17" s="64"/>
-      <c r="O17" s="64"/>
-      <c r="P17" s="64"/>
-      <c r="Q17" s="64"/>
-      <c r="R17" s="64"/>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A18" s="38" t="s">
-        <v>71</v>
       </c>
       <c r="B18" s="45">
         <v>1E-3</v>
       </c>
       <c r="C18" s="40" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D18" s="41" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E18" s="42"/>
       <c r="F18" s="43"/>
       <c r="G18" s="25" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H18" s="48" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I18" s="7"/>
-      <c r="J18" s="64" t="s">
-        <v>89</v>
-      </c>
-      <c r="K18" s="64"/>
-      <c r="L18" s="64"/>
-      <c r="M18" s="64"/>
-      <c r="N18" s="64"/>
-      <c r="O18" s="64"/>
-      <c r="P18" s="64"/>
-      <c r="Q18" s="64"/>
-      <c r="R18" s="64"/>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="J18" s="56" t="s">
+        <v>87</v>
+      </c>
+      <c r="K18" s="56"/>
+      <c r="L18" s="56"/>
+      <c r="M18" s="56"/>
+      <c r="N18" s="56"/>
+      <c r="O18" s="56"/>
+      <c r="P18" s="56"/>
+      <c r="Q18" s="56"/>
+      <c r="R18" s="56"/>
+    </row>
+    <row r="19" spans="1:18">
       <c r="G19" s="46"/>
       <c r="H19" s="7"/>
       <c r="I19" s="7"/>
@@ -1667,7 +1707,7 @@
       <c r="Q19" s="53"/>
       <c r="R19" s="54"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:18">
       <c r="G20" s="46"/>
       <c r="H20" s="7"/>
       <c r="I20" s="7"/>
@@ -1681,17 +1721,17 @@
       <c r="Q20" s="53"/>
       <c r="R20" s="54"/>
     </row>
-    <row r="21" spans="1:18" ht="19" x14ac:dyDescent="0.2">
-      <c r="A21" s="59" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" s="59"/>
-      <c r="C21" s="59"/>
-      <c r="D21" s="60"/>
-      <c r="G21" s="61" t="s">
-        <v>24</v>
-      </c>
-      <c r="H21" s="60"/>
+    <row r="21" spans="1:18" ht="18.75">
+      <c r="A21" s="67" t="s">
+        <v>95</v>
+      </c>
+      <c r="B21" s="67"/>
+      <c r="C21" s="67"/>
+      <c r="D21" s="63"/>
+      <c r="G21" s="62" t="s">
+        <v>95</v>
+      </c>
+      <c r="H21" s="63"/>
       <c r="I21" s="7"/>
       <c r="J21" s="52"/>
       <c r="K21" s="53"/>
@@ -1703,7 +1743,7 @@
       <c r="Q21" s="53"/>
       <c r="R21" s="54"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:18">
       <c r="G22" s="46"/>
       <c r="H22" s="7"/>
       <c r="I22" s="7"/>
@@ -1717,7 +1757,7 @@
       <c r="Q22" s="53"/>
       <c r="R22" s="54"/>
     </row>
-    <row r="23" spans="1:18" ht="19" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:18" ht="18.75">
       <c r="G23" s="46"/>
       <c r="H23" s="7"/>
       <c r="I23" s="51"/>
@@ -1731,81 +1771,99 @@
       <c r="Q23" s="53"/>
       <c r="R23" s="54"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:18">
       <c r="A24" s="30" t="s">
-        <v>8</v>
+        <v>96</v>
       </c>
       <c r="B24" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="G24" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="H24" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="I24" s="7"/>
+      <c r="J24" s="60" t="s">
+        <v>15</v>
+      </c>
+      <c r="K24" s="60"/>
+      <c r="L24" s="60"/>
+      <c r="M24" s="60"/>
+      <c r="N24" s="60"/>
+      <c r="O24" s="60"/>
+      <c r="P24" s="60"/>
+      <c r="Q24" s="60"/>
+      <c r="R24" s="60"/>
+    </row>
+    <row r="25" spans="1:18">
+      <c r="A25" s="68"/>
+      <c r="B25" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="G25" s="69"/>
+      <c r="H25" s="43" t="s">
+        <v>98</v>
+      </c>
+      <c r="I25" s="7"/>
+      <c r="J25" s="70" t="s">
+        <v>15</v>
+      </c>
+      <c r="K25" s="71"/>
+      <c r="L25" s="71"/>
+      <c r="M25" s="71"/>
+      <c r="N25" s="71"/>
+      <c r="O25" s="71"/>
+      <c r="P25" s="71"/>
+      <c r="Q25" s="71"/>
+      <c r="R25" s="72"/>
+    </row>
+    <row r="26" spans="1:18">
+      <c r="A26" s="31"/>
+      <c r="B26" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C24" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D24" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="G24" s="28" t="s">
-        <v>40</v>
-      </c>
-      <c r="H24" s="43" t="s">
+      <c r="C26" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="G26" s="29"/>
+      <c r="H26" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="I24" s="7"/>
-      <c r="J24" s="67"/>
-      <c r="K24" s="67"/>
-      <c r="L24" s="67"/>
-      <c r="M24" s="67"/>
-      <c r="N24" s="67"/>
-      <c r="O24" s="67"/>
-      <c r="P24" s="67"/>
-      <c r="Q24" s="67"/>
-      <c r="R24" s="67"/>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A25" s="31"/>
-      <c r="B25" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C25" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="G25" s="29"/>
-      <c r="H25" s="43" t="s">
-        <v>22</v>
-      </c>
-      <c r="I25" s="7"/>
-      <c r="J25" s="67"/>
-      <c r="K25" s="67"/>
-      <c r="L25" s="67"/>
-      <c r="M25" s="67"/>
-      <c r="N25" s="67"/>
-      <c r="O25" s="67"/>
-      <c r="P25" s="67"/>
-      <c r="Q25" s="67"/>
-      <c r="R25" s="67"/>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A26" s="18"/>
-      <c r="B26" s="18"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="22"/>
-      <c r="G26" s="46"/>
-      <c r="H26" s="7"/>
       <c r="I26" s="7"/>
-      <c r="J26" s="52"/>
-      <c r="K26" s="53"/>
-      <c r="L26" s="53"/>
-      <c r="M26" s="53"/>
-      <c r="N26" s="53"/>
-      <c r="O26" s="53"/>
-      <c r="P26" s="53"/>
-      <c r="Q26" s="53"/>
-      <c r="R26" s="54"/>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="J26" s="60" t="s">
+        <v>15</v>
+      </c>
+      <c r="K26" s="60"/>
+      <c r="L26" s="60"/>
+      <c r="M26" s="60"/>
+      <c r="N26" s="60"/>
+      <c r="O26" s="60"/>
+      <c r="P26" s="60"/>
+      <c r="Q26" s="60"/>
+      <c r="R26" s="60"/>
+    </row>
+    <row r="27" spans="1:18">
+      <c r="A27" s="18"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="22"/>
       <c r="G27" s="46"/>
       <c r="H27" s="7"/>
       <c r="I27" s="7"/>
@@ -1819,199 +1877,231 @@
       <c r="Q27" s="53"/>
       <c r="R27" s="54"/>
     </row>
-    <row r="28" spans="1:18" ht="19" x14ac:dyDescent="0.2">
-      <c r="A28" s="63" t="s">
-        <v>72</v>
-      </c>
-      <c r="B28" s="63"/>
-      <c r="C28" s="63"/>
-      <c r="D28" s="60"/>
-      <c r="G28" s="61" t="s">
-        <v>72</v>
-      </c>
-      <c r="H28" s="60"/>
-      <c r="I28" s="51"/>
-      <c r="J28" s="52"/>
-      <c r="K28" s="53"/>
-      <c r="L28" s="53"/>
-      <c r="M28" s="53"/>
-      <c r="N28" s="53"/>
-      <c r="O28" s="53"/>
-      <c r="P28" s="53"/>
-      <c r="Q28" s="53"/>
-      <c r="R28" s="54"/>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A29" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B29" s="10">
+    <row r="28" spans="1:18">
+      <c r="A28" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="G28" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="H28" s="43" t="s">
+        <v>103</v>
+      </c>
+      <c r="I28" s="7"/>
+      <c r="J28" s="60" t="s">
+        <v>15</v>
+      </c>
+      <c r="K28" s="60"/>
+      <c r="L28" s="60"/>
+      <c r="M28" s="60"/>
+      <c r="N28" s="60"/>
+      <c r="O28" s="60"/>
+      <c r="P28" s="60"/>
+      <c r="Q28" s="60"/>
+      <c r="R28" s="60"/>
+    </row>
+    <row r="29" spans="1:18">
+      <c r="A29" s="31"/>
+      <c r="B29" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="C29" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="G29" s="29"/>
+      <c r="H29" s="43" t="s">
+        <v>104</v>
+      </c>
+      <c r="I29" s="7"/>
+      <c r="J29" s="70" t="s">
+        <v>15</v>
+      </c>
+      <c r="K29" s="71"/>
+      <c r="L29" s="71"/>
+      <c r="M29" s="71"/>
+      <c r="N29" s="71"/>
+      <c r="O29" s="71"/>
+      <c r="P29" s="71"/>
+      <c r="Q29" s="71"/>
+      <c r="R29" s="72"/>
+    </row>
+    <row r="30" spans="1:18">
+      <c r="G30" s="46"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="52"/>
+      <c r="K30" s="53"/>
+      <c r="L30" s="53"/>
+      <c r="M30" s="53"/>
+      <c r="N30" s="53"/>
+      <c r="O30" s="53"/>
+      <c r="P30" s="53"/>
+      <c r="Q30" s="53"/>
+      <c r="R30" s="54"/>
+    </row>
+    <row r="31" spans="1:18" ht="18.75">
+      <c r="A31" s="64" t="s">
+        <v>70</v>
+      </c>
+      <c r="B31" s="64"/>
+      <c r="C31" s="64"/>
+      <c r="D31" s="63"/>
+      <c r="G31" s="62" t="s">
+        <v>70</v>
+      </c>
+      <c r="H31" s="63"/>
+      <c r="I31" s="51"/>
+      <c r="J31" s="52"/>
+      <c r="K31" s="53"/>
+      <c r="L31" s="53"/>
+      <c r="M31" s="53"/>
+      <c r="N31" s="53"/>
+      <c r="O31" s="53"/>
+      <c r="P31" s="53"/>
+      <c r="Q31" s="53"/>
+      <c r="R31" s="54"/>
+    </row>
+    <row r="32" spans="1:18">
+      <c r="A32" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B32" s="10">
         <v>550</v>
       </c>
-      <c r="C29" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D29" s="13" t="s">
+      <c r="C32" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="G32" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="H32" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="I32" s="7"/>
+      <c r="J32" s="56" t="s">
+        <v>88</v>
+      </c>
+      <c r="K32" s="56"/>
+      <c r="L32" s="56"/>
+      <c r="M32" s="56"/>
+      <c r="N32" s="56"/>
+      <c r="O32" s="56"/>
+      <c r="P32" s="56"/>
+      <c r="Q32" s="56"/>
+      <c r="R32" s="56"/>
+    </row>
+    <row r="33" spans="1:18">
+      <c r="A33" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B33" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="C33" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G33" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="H33" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="I33" s="7"/>
+      <c r="J33" s="56" t="s">
+        <v>89</v>
+      </c>
+      <c r="K33" s="56"/>
+      <c r="L33" s="56"/>
+      <c r="M33" s="56"/>
+      <c r="N33" s="56"/>
+      <c r="O33" s="56"/>
+      <c r="P33" s="56"/>
+      <c r="Q33" s="56"/>
+      <c r="R33" s="56"/>
+    </row>
+    <row r="34" spans="1:18">
+      <c r="A34" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="G29" s="24" t="s">
+      <c r="B34" s="18">
+        <v>5</v>
+      </c>
+      <c r="C34" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="G34" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="H29" s="36" t="s">
-        <v>38</v>
-      </c>
-      <c r="I29" s="7"/>
-      <c r="J29" s="64" t="s">
+      <c r="H34" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="I34" s="7"/>
+      <c r="J34" s="56" t="s">
         <v>90</v>
       </c>
-      <c r="K29" s="64"/>
-      <c r="L29" s="64"/>
-      <c r="M29" s="64"/>
-      <c r="N29" s="64"/>
-      <c r="O29" s="64"/>
-      <c r="P29" s="64"/>
-      <c r="Q29" s="64"/>
-      <c r="R29" s="64"/>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A30" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="B30" s="14">
+      <c r="K34" s="56"/>
+      <c r="L34" s="56"/>
+      <c r="M34" s="56"/>
+      <c r="N34" s="56"/>
+      <c r="O34" s="56"/>
+      <c r="P34" s="56"/>
+      <c r="Q34" s="56"/>
+      <c r="R34" s="56"/>
+    </row>
+    <row r="35" spans="1:18">
+      <c r="A35" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B35" s="14">
         <v>0.1</v>
       </c>
-      <c r="C30" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D30" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="G30" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="H30" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="I30" s="7"/>
-      <c r="J30" s="64" t="s">
-        <v>91</v>
-      </c>
-      <c r="K30" s="64"/>
-      <c r="L30" s="64"/>
-      <c r="M30" s="64"/>
-      <c r="N30" s="64"/>
-      <c r="O30" s="64"/>
-      <c r="P30" s="64"/>
-      <c r="Q30" s="64"/>
-      <c r="R30" s="64"/>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A31" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="B31" s="18">
-        <v>5</v>
-      </c>
-      <c r="C31" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="G31" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="H31" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="I31" s="7"/>
-      <c r="J31" s="64" t="s">
-        <v>92</v>
-      </c>
-      <c r="K31" s="64"/>
-      <c r="L31" s="64"/>
-      <c r="M31" s="64"/>
-      <c r="N31" s="64"/>
-      <c r="O31" s="64"/>
-      <c r="P31" s="64"/>
-      <c r="Q31" s="64"/>
-      <c r="R31" s="64"/>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A32" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="B32" s="14">
-        <v>0.1</v>
-      </c>
-      <c r="C32" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="D32" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="G32" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="H32" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="I32" s="7"/>
-      <c r="J32" s="64" t="s">
-        <v>96</v>
-      </c>
-      <c r="K32" s="64"/>
-      <c r="L32" s="64"/>
-      <c r="M32" s="64"/>
-      <c r="N32" s="64"/>
-      <c r="O32" s="64"/>
-      <c r="P32" s="64"/>
-      <c r="Q32" s="64"/>
-      <c r="R32" s="64"/>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="G33" s="46"/>
-      <c r="H33" s="7"/>
-      <c r="I33" s="7"/>
-      <c r="J33" s="52"/>
-      <c r="K33" s="53"/>
-      <c r="L33" s="53"/>
-      <c r="M33" s="53"/>
-      <c r="N33" s="53"/>
-      <c r="O33" s="53"/>
-      <c r="P33" s="53"/>
-      <c r="Q33" s="53"/>
-      <c r="R33" s="54"/>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="G34" s="46"/>
-      <c r="H34" s="7"/>
-      <c r="I34" s="7"/>
-      <c r="J34" s="52"/>
-      <c r="K34" s="53"/>
-      <c r="L34" s="53"/>
-      <c r="M34" s="53"/>
-      <c r="N34" s="53"/>
-      <c r="O34" s="53"/>
-      <c r="P34" s="53"/>
-      <c r="Q34" s="53"/>
-      <c r="R34" s="54"/>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="G35" s="46"/>
-      <c r="H35" s="7"/>
+      <c r="C35" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D35" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="G35" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="H35" s="43" t="s">
+        <v>15</v>
+      </c>
       <c r="I35" s="7"/>
-      <c r="J35" s="52"/>
-      <c r="K35" s="53"/>
-      <c r="L35" s="53"/>
-      <c r="M35" s="53"/>
-      <c r="N35" s="53"/>
-      <c r="O35" s="53"/>
-      <c r="P35" s="53"/>
-      <c r="Q35" s="53"/>
-      <c r="R35" s="54"/>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="J35" s="56" t="s">
+        <v>94</v>
+      </c>
+      <c r="K35" s="56"/>
+      <c r="L35" s="56"/>
+      <c r="M35" s="56"/>
+      <c r="N35" s="56"/>
+      <c r="O35" s="56"/>
+      <c r="P35" s="56"/>
+      <c r="Q35" s="56"/>
+      <c r="R35" s="56"/>
+    </row>
+    <row r="36" spans="1:18">
       <c r="G36" s="46"/>
       <c r="H36" s="7"/>
       <c r="I36" s="7"/>
@@ -2025,17 +2115,9 @@
       <c r="Q36" s="53"/>
       <c r="R36" s="54"/>
     </row>
-    <row r="37" spans="1:18" ht="19" x14ac:dyDescent="0.2">
-      <c r="A37" s="63" t="s">
-        <v>73</v>
-      </c>
-      <c r="B37" s="63"/>
-      <c r="C37" s="63"/>
-      <c r="D37" s="60"/>
-      <c r="G37" s="61" t="s">
-        <v>73</v>
-      </c>
-      <c r="H37" s="60"/>
+    <row r="37" spans="1:18">
+      <c r="G37" s="46"/>
+      <c r="H37" s="7"/>
       <c r="I37" s="7"/>
       <c r="J37" s="52"/>
       <c r="K37" s="53"/>
@@ -2047,214 +2129,254 @@
       <c r="Q37" s="53"/>
       <c r="R37" s="54"/>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A38" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B38" s="10">
+    <row r="38" spans="1:18">
+      <c r="G38" s="46"/>
+      <c r="H38" s="7"/>
+      <c r="I38" s="7"/>
+      <c r="J38" s="52"/>
+      <c r="K38" s="53"/>
+      <c r="L38" s="53"/>
+      <c r="M38" s="53"/>
+      <c r="N38" s="53"/>
+      <c r="O38" s="53"/>
+      <c r="P38" s="53"/>
+      <c r="Q38" s="53"/>
+      <c r="R38" s="54"/>
+    </row>
+    <row r="39" spans="1:18">
+      <c r="G39" s="46"/>
+      <c r="H39" s="7"/>
+      <c r="I39" s="7"/>
+      <c r="J39" s="52"/>
+      <c r="K39" s="53"/>
+      <c r="L39" s="53"/>
+      <c r="M39" s="53"/>
+      <c r="N39" s="53"/>
+      <c r="O39" s="53"/>
+      <c r="P39" s="53"/>
+      <c r="Q39" s="53"/>
+      <c r="R39" s="54"/>
+    </row>
+    <row r="40" spans="1:18" ht="18.75">
+      <c r="A40" s="64" t="s">
+        <v>71</v>
+      </c>
+      <c r="B40" s="64"/>
+      <c r="C40" s="64"/>
+      <c r="D40" s="63"/>
+      <c r="G40" s="62" t="s">
+        <v>71</v>
+      </c>
+      <c r="H40" s="63"/>
+      <c r="I40" s="7"/>
+      <c r="J40" s="52"/>
+      <c r="K40" s="53"/>
+      <c r="L40" s="53"/>
+      <c r="M40" s="53"/>
+      <c r="N40" s="53"/>
+      <c r="O40" s="53"/>
+      <c r="P40" s="53"/>
+      <c r="Q40" s="53"/>
+      <c r="R40" s="54"/>
+    </row>
+    <row r="41" spans="1:18">
+      <c r="A41" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B41" s="10">
         <v>550</v>
       </c>
-      <c r="C38" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D38" s="13" t="s">
+      <c r="C41" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D41" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="G41" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="H41" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="I41" s="7"/>
+      <c r="J41" s="56" t="s">
+        <v>91</v>
+      </c>
+      <c r="K41" s="56"/>
+      <c r="L41" s="56"/>
+      <c r="M41" s="56"/>
+      <c r="N41" s="56"/>
+      <c r="O41" s="56"/>
+      <c r="P41" s="56"/>
+      <c r="Q41" s="56"/>
+      <c r="R41" s="56"/>
+    </row>
+    <row r="42" spans="1:18">
+      <c r="A42" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B42" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="C42" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D42" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G42" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="H42" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="I42" s="7"/>
+      <c r="J42" s="56" t="s">
+        <v>92</v>
+      </c>
+      <c r="K42" s="56"/>
+      <c r="L42" s="56"/>
+      <c r="M42" s="56"/>
+      <c r="N42" s="56"/>
+      <c r="O42" s="56"/>
+      <c r="P42" s="56"/>
+      <c r="Q42" s="56"/>
+      <c r="R42" s="56"/>
+    </row>
+    <row r="43" spans="1:18">
+      <c r="A43" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="G38" s="24" t="s">
+      <c r="B43" s="18">
+        <v>5</v>
+      </c>
+      <c r="C43" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D43" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="G43" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="H38" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="I38" s="7"/>
-      <c r="J38" s="64" t="s">
+      <c r="H43" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="I43" s="7"/>
+      <c r="J43" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="K38" s="64"/>
-      <c r="L38" s="64"/>
-      <c r="M38" s="64"/>
-      <c r="N38" s="64"/>
-      <c r="O38" s="64"/>
-      <c r="P38" s="64"/>
-      <c r="Q38" s="64"/>
-      <c r="R38" s="64"/>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A39" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="B39" s="14">
+      <c r="K43" s="56"/>
+      <c r="L43" s="56"/>
+      <c r="M43" s="56"/>
+      <c r="N43" s="56"/>
+      <c r="O43" s="56"/>
+      <c r="P43" s="56"/>
+      <c r="Q43" s="56"/>
+      <c r="R43" s="56"/>
+    </row>
+    <row r="44" spans="1:18">
+      <c r="A44" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B44" s="14">
         <v>0.1</v>
       </c>
-      <c r="C39" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D39" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="G39" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="H39" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="I39" s="7"/>
-      <c r="J39" s="64" t="s">
+      <c r="C44" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D44" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="G44" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="H44" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="I44" s="7"/>
+      <c r="J44" s="56" t="s">
         <v>94</v>
       </c>
-      <c r="K39" s="64"/>
-      <c r="L39" s="64"/>
-      <c r="M39" s="64"/>
-      <c r="N39" s="64"/>
-      <c r="O39" s="64"/>
-      <c r="P39" s="64"/>
-      <c r="Q39" s="64"/>
-      <c r="R39" s="64"/>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A40" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="B40" s="18">
-        <v>5</v>
-      </c>
-      <c r="C40" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="D40" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="G40" s="26" t="s">
-        <v>52</v>
-      </c>
-      <c r="H40" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="I40" s="7"/>
-      <c r="J40" s="64" t="s">
-        <v>95</v>
-      </c>
-      <c r="K40" s="64"/>
-      <c r="L40" s="64"/>
-      <c r="M40" s="64"/>
-      <c r="N40" s="64"/>
-      <c r="O40" s="64"/>
-      <c r="P40" s="64"/>
-      <c r="Q40" s="64"/>
-      <c r="R40" s="64"/>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A41" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="B41" s="14">
-        <v>0.1</v>
-      </c>
-      <c r="C41" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="D41" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="G41" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="H41" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="I41" s="7"/>
-      <c r="J41" s="64" t="s">
-        <v>96</v>
-      </c>
-      <c r="K41" s="64"/>
-      <c r="L41" s="64"/>
-      <c r="M41" s="64"/>
-      <c r="N41" s="64"/>
-      <c r="O41" s="64"/>
-      <c r="P41" s="64"/>
-      <c r="Q41" s="64"/>
-      <c r="R41" s="64"/>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="I42" s="7"/>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="I43" s="7"/>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="I44" s="7"/>
-    </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="K44" s="56"/>
+      <c r="L44" s="56"/>
+      <c r="M44" s="56"/>
+      <c r="N44" s="56"/>
+      <c r="O44" s="56"/>
+      <c r="P44" s="56"/>
+      <c r="Q44" s="56"/>
+      <c r="R44" s="56"/>
+    </row>
+    <row r="45" spans="1:18">
       <c r="I45" s="7"/>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:18">
       <c r="I46" s="7"/>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:18">
       <c r="I47" s="7"/>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:18">
       <c r="I48" s="7"/>
     </row>
-    <row r="49" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="9:9">
       <c r="I49" s="7"/>
     </row>
-    <row r="50" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="50" spans="9:9">
       <c r="I50" s="7"/>
     </row>
-    <row r="51" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="9:9">
       <c r="I51" s="7"/>
     </row>
-    <row r="52" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="9:9">
       <c r="I52" s="7"/>
     </row>
-    <row r="53" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="53" spans="9:9">
       <c r="I53" s="7"/>
     </row>
-    <row r="54" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="54" spans="9:9">
       <c r="I54" s="7"/>
     </row>
-    <row r="55" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="55" spans="9:9">
       <c r="I55" s="7"/>
     </row>
-    <row r="56" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="56" spans="9:9">
       <c r="I56" s="7"/>
     </row>
-    <row r="57" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="57" spans="9:9">
       <c r="I57" s="7"/>
     </row>
-    <row r="58" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="58" spans="9:9">
       <c r="I58" s="7"/>
     </row>
-    <row r="59" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="59" spans="9:9">
       <c r="I59" s="7"/>
     </row>
-    <row r="60" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="60" spans="9:9">
       <c r="I60" s="7"/>
     </row>
+    <row r="61" spans="9:9">
+      <c r="I61" s="7"/>
+    </row>
+    <row r="62" spans="9:9">
+      <c r="I62" s="7"/>
+    </row>
+    <row r="63" spans="9:9">
+      <c r="I63" s="7"/>
+    </row>
   </sheetData>
-  <mergeCells count="35">
-    <mergeCell ref="J39:R39"/>
-    <mergeCell ref="J40:R40"/>
-    <mergeCell ref="J41:R41"/>
-    <mergeCell ref="J1:R1"/>
-    <mergeCell ref="J2:R2"/>
-    <mergeCell ref="J30:R30"/>
-    <mergeCell ref="J31:R31"/>
-    <mergeCell ref="J32:R32"/>
-    <mergeCell ref="J38:R38"/>
-    <mergeCell ref="J17:R17"/>
-    <mergeCell ref="J18:R18"/>
-    <mergeCell ref="J24:R24"/>
-    <mergeCell ref="J25:R25"/>
-    <mergeCell ref="J29:R29"/>
-    <mergeCell ref="J12:R12"/>
-    <mergeCell ref="J13:R13"/>
+  <mergeCells count="38">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G21:H21"/>
     <mergeCell ref="J6:R6"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="A40:D40"/>
     <mergeCell ref="J14:R14"/>
     <mergeCell ref="J15:R15"/>
     <mergeCell ref="J16:R16"/>
@@ -2263,12 +2385,25 @@
     <mergeCell ref="J9:R9"/>
     <mergeCell ref="J10:R10"/>
     <mergeCell ref="J11:R11"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="J25:R25"/>
+    <mergeCell ref="J28:R28"/>
+    <mergeCell ref="J29:R29"/>
+    <mergeCell ref="J42:R42"/>
+    <mergeCell ref="J43:R43"/>
+    <mergeCell ref="J44:R44"/>
+    <mergeCell ref="J1:R1"/>
+    <mergeCell ref="J2:R2"/>
+    <mergeCell ref="J33:R33"/>
+    <mergeCell ref="J34:R34"/>
+    <mergeCell ref="J35:R35"/>
+    <mergeCell ref="J41:R41"/>
+    <mergeCell ref="J17:R17"/>
+    <mergeCell ref="J18:R18"/>
+    <mergeCell ref="J24:R24"/>
+    <mergeCell ref="J26:R26"/>
+    <mergeCell ref="J32:R32"/>
+    <mergeCell ref="J12:R12"/>
+    <mergeCell ref="J13:R13"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>